<commit_message>
1. Added Email Notification after Run 2. Screenshot in report changed to Base 64
</commit_message>
<xml_diff>
--- a/src/main/resources/com/kh/PRISM/TestData/TestData.xlsx
+++ b/src/main/resources/com/kh/PRISM/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdityaPrasad\Desktop\SeleniumScript\IRA\src\main\resources\com\kh\PRISM\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdityaPrasad\Desktop\SeleniumScript\PRISM\src\main\resources\com\kh\PRISM\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35889882-AF64-41D2-AD3B-6F20FFDE4C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693A2B2C-20AD-4450-9425-F20BE8B74EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>